<commit_message>
[FIXED] - Revision 01
</commit_message>
<xml_diff>
--- a/data/indicadores_relevantes.xlsx
+++ b/data/indicadores_relevantes.xlsx
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Datos</t>
   </si>
   <si>
-    <t xml:space="preserve">M2 de GLA&lt;br&gt;(Propias y Administradas)</t>
+    <t xml:space="preserve">de GLA&lt;br&gt;(Propias y Administradas)</t>
   </si>
   <si>
     <t xml:space="preserve">93.9%</t>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
added - new plani reports 4th 2023
</commit_message>
<xml_diff>
--- a/data/indicadores_relevantes.xlsx
+++ b/data/indicadores_relevantes.xlsx
@@ -31,13 +31,13 @@
     <t xml:space="preserve">Espacio Comercial (GLA)</t>
   </si>
   <si>
-    <t xml:space="preserve">93.9%</t>
+    <t xml:space="preserve">93.7%</t>
   </si>
   <si>
     <t xml:space="preserve">de Ocupación &lt;br&gt;(Propias y Administradas)</t>
   </si>
   <si>
-    <t xml:space="preserve">+2,000</t>
+    <t xml:space="preserve">+2,500</t>
   </si>
   <si>
     <t xml:space="preserve">Contratos de &lt;br&gt; Arrendamiento</t>
@@ -46,7 +46,7 @@
     <t xml:space="preserve">Inquilinos &lt;br&gt; AAA</t>
   </si>
   <si>
-    <t xml:space="preserve">+26,3 Millones</t>
+    <t xml:space="preserve">+27,0 Millones</t>
   </si>
   <si>
     <t xml:space="preserve">Visitantes al 3T2023&lt;br&gt;(Propias y Administradas)</t>
@@ -443,7 +443,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>